<commit_message>
Added funtionality that scrapes covid-19 mortality from the ministry of health in Bulgaria.
</commit_message>
<xml_diff>
--- a/data_output/Excess Mortality/Regions/TOTAL_BG_Total_['Female', 'Male', 'Total']_excess_mortality_2020.xlsx
+++ b/data_output/Excess Mortality/Regions/TOTAL_BG_Total_['Female', 'Male', 'Total']_excess_mortality_2020.xlsx
@@ -662,7 +662,7 @@
         <v>2020</v>
       </c>
       <c r="D3" t="n">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="E3" t="n">
         <v>2133</v>
@@ -698,7 +698,7 @@
         <v>2174.5</v>
       </c>
       <c r="P3" t="n">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q3" t="n">
         <v>28.5</v>
@@ -716,7 +716,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>310.0 (±28.5)</t>
+          <t>309.0 (±28.5)</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -728,14 +728,14 @@
         <v>211475</v>
       </c>
       <c r="X3" t="n">
-        <v>146.6</v>
+        <v>146.1</v>
       </c>
       <c r="Y3" t="n">
         <v>13.5</v>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>146.6(±13.5)</t>
+          <t>146.1(±13.5)</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
         <v>2020</v>
       </c>
       <c r="D6" t="n">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="E6" t="n">
         <v>1581</v>
@@ -974,13 +974,13 @@
         <v>1547.7</v>
       </c>
       <c r="P6" t="n">
-        <v>252.6</v>
+        <v>253.6</v>
       </c>
       <c r="Q6" t="n">
         <v>55.3</v>
       </c>
       <c r="R6" t="n">
-        <v>16.9</v>
+        <v>17</v>
       </c>
       <c r="S6" t="n">
         <v>4.2</v>
@@ -992,26 +992,26 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>252.6 (±55.3)</t>
+          <t>253.6 (±55.3)</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>16.9% (±4.2%)</t>
+          <t>17.0% (±4.2%)</t>
         </is>
       </c>
       <c r="W6" t="n">
         <v>115346</v>
       </c>
       <c r="X6" t="n">
-        <v>219</v>
+        <v>219.9</v>
       </c>
       <c r="Y6" t="n">
         <v>47.9</v>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>219.0(±47.9)</t>
+          <t>219.9(±47.9)</t>
         </is>
       </c>
     </row>
@@ -1306,7 +1306,7 @@
         <v>2020</v>
       </c>
       <c r="D10" t="n">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="E10" t="n">
         <v>1177</v>
@@ -1342,13 +1342,13 @@
         <v>1161.6</v>
       </c>
       <c r="P10" t="n">
-        <v>121.6</v>
+        <v>122.6</v>
       </c>
       <c r="Q10" t="n">
         <v>32.2</v>
       </c>
       <c r="R10" t="n">
-        <v>10.8</v>
+        <v>10.9</v>
       </c>
       <c r="S10" t="n">
         <v>3.1</v>
@@ -1360,26 +1360,26 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>121.6 (±32.2)</t>
+          <t>122.6 (±32.2)</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>10.8% (±3.1%)</t>
+          <t>10.9% (±3.1%)</t>
         </is>
       </c>
       <c r="W10" t="n">
         <v>64880</v>
       </c>
       <c r="X10" t="n">
-        <v>187.4</v>
+        <v>189</v>
       </c>
       <c r="Y10" t="n">
-        <v>49.7</v>
+        <v>49.6</v>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>187.4(±49.7)</t>
+          <t>189.0(±49.6)</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
         <v>2020</v>
       </c>
       <c r="D11" t="n">
-        <v>1908</v>
+        <v>1909</v>
       </c>
       <c r="E11" t="n">
         <v>1604</v>
@@ -1434,16 +1434,16 @@
         <v>1605.1</v>
       </c>
       <c r="P11" t="n">
-        <v>349.2</v>
+        <v>350.2</v>
       </c>
       <c r="Q11" t="n">
         <v>46.3</v>
       </c>
       <c r="R11" t="n">
-        <v>22.4</v>
+        <v>22.5</v>
       </c>
       <c r="S11" t="n">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -1452,26 +1452,26 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>349.2 (±46.3)</t>
+          <t>350.2 (±46.3)</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>22.4% (±3.5%)</t>
+          <t>22.5% (±3.6%)</t>
         </is>
       </c>
       <c r="W11" t="n">
         <v>129061</v>
       </c>
       <c r="X11" t="n">
-        <v>270.6</v>
+        <v>271.3</v>
       </c>
       <c r="Y11" t="n">
-        <v>35.8</v>
+        <v>35.9</v>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>270.6(±35.8)</t>
+          <t>271.3(±35.9)</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1674,7 @@
         <v>2020</v>
       </c>
       <c r="D14" t="n">
-        <v>4724</v>
+        <v>4723</v>
       </c>
       <c r="E14" t="n">
         <v>3901</v>
@@ -1710,7 +1710,7 @@
         <v>3940.199999999999</v>
       </c>
       <c r="P14" t="n">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="Q14" t="n">
         <v>71.2</v>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>855.0 (±71.2)</t>
+          <t>854.0 (±71.2)</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
@@ -1740,14 +1740,14 @@
         <v>346665</v>
       </c>
       <c r="X14" t="n">
-        <v>246.6</v>
+        <v>246.3</v>
       </c>
       <c r="Y14" t="n">
         <v>20.6</v>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>246.6(±20.6)</t>
+          <t>246.3(±20.6)</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
         <v>2020</v>
       </c>
       <c r="D15" t="n">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="E15" t="n">
         <v>743</v>
@@ -1802,13 +1802,13 @@
         <v>749.9000000000001</v>
       </c>
       <c r="P15" t="n">
-        <v>213.4</v>
+        <v>214.4</v>
       </c>
       <c r="Q15" t="n">
         <v>19.3</v>
       </c>
       <c r="R15" t="n">
-        <v>29.2</v>
+        <v>29.3</v>
       </c>
       <c r="S15" t="n">
         <v>3.3</v>
@@ -1820,26 +1820,26 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>213.4 (±19.3)</t>
+          <t>214.4 (±19.3)</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>29.2% (±3.3%)</t>
+          <t>29.3% (±3.3%)</t>
         </is>
       </c>
       <c r="W15" t="n">
         <v>56777</v>
       </c>
       <c r="X15" t="n">
-        <v>375.9</v>
+        <v>377.6</v>
       </c>
       <c r="Y15" t="n">
-        <v>33.9</v>
+        <v>34</v>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>375.9(±33.9)</t>
+          <t>377.6(±34.0)</t>
         </is>
       </c>
     </row>
@@ -2134,7 +2134,7 @@
         <v>2020</v>
       </c>
       <c r="D19" t="n">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="E19" t="n">
         <v>1168</v>
@@ -2170,16 +2170,16 @@
         <v>1136.2</v>
       </c>
       <c r="P19" t="n">
-        <v>267.6</v>
+        <v>268.6</v>
       </c>
       <c r="Q19" t="n">
         <v>40.8</v>
       </c>
       <c r="R19" t="n">
-        <v>24.4</v>
+        <v>24.5</v>
       </c>
       <c r="S19" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
@@ -2188,26 +2188,26 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>267.6 (±40.8)</t>
+          <t>268.6 (±40.8)</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>24.4% (±4.4%)</t>
+          <t>24.5% (±4.5%)</t>
         </is>
       </c>
       <c r="W19" t="n">
         <v>94697</v>
       </c>
       <c r="X19" t="n">
-        <v>282.6</v>
+        <v>283.6</v>
       </c>
       <c r="Y19" t="n">
         <v>43.1</v>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>282.6(±43.1)</t>
+          <t>283.6(±43.1)</t>
         </is>
       </c>
     </row>
@@ -2410,7 +2410,7 @@
         <v>2020</v>
       </c>
       <c r="D22" t="n">
-        <v>7283</v>
+        <v>7288</v>
       </c>
       <c r="E22" t="n">
         <v>6564</v>
@@ -2446,16 +2446,16 @@
         <v>6586.600000000002</v>
       </c>
       <c r="P22" t="n">
-        <v>802</v>
+        <v>807</v>
       </c>
       <c r="Q22" t="n">
         <v>105.6</v>
       </c>
       <c r="R22" t="n">
-        <v>12.4</v>
+        <v>12.5</v>
       </c>
       <c r="S22" t="n">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
@@ -2464,26 +2464,26 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>802.0 (±105.6)</t>
+          <t>807.0 (±105.6)</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>12.4% (±1.8%)</t>
+          <t>12.5% (±1.9%)</t>
         </is>
       </c>
       <c r="W22" t="n">
         <v>691325</v>
       </c>
       <c r="X22" t="n">
-        <v>116</v>
+        <v>116.7</v>
       </c>
       <c r="Y22" t="n">
         <v>15.3</v>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>116.0(±15.3)</t>
+          <t>116.7(±15.3)</t>
         </is>
       </c>
     </row>
@@ -2594,7 +2594,7 @@
         <v>2020</v>
       </c>
       <c r="D24" t="n">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="E24" t="n">
         <v>704</v>
@@ -2630,13 +2630,13 @@
         <v>745.5</v>
       </c>
       <c r="P24" t="n">
-        <v>157.4</v>
+        <v>158.4</v>
       </c>
       <c r="Q24" t="n">
         <v>13.9</v>
       </c>
       <c r="R24" t="n">
-        <v>21.5</v>
+        <v>21.7</v>
       </c>
       <c r="S24" t="n">
         <v>2.3</v>
@@ -2648,26 +2648,26 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>157.4 (±13.9)</t>
+          <t>158.4 (±13.9)</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>21.5% (±2.3%)</t>
+          <t>21.7% (±2.3%)</t>
         </is>
       </c>
       <c r="W24" t="n">
         <v>56750</v>
       </c>
       <c r="X24" t="n">
-        <v>277.4</v>
+        <v>279.1</v>
       </c>
       <c r="Y24" t="n">
         <v>24.5</v>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>277.4(±24.5)</t>
+          <t>279.1(±24.5)</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3238,7 @@
         <v>2020</v>
       </c>
       <c r="D31" t="n">
-        <v>2807</v>
+        <v>2808</v>
       </c>
       <c r="E31" t="n">
         <v>2406</v>
@@ -3274,7 +3274,7 @@
         <v>2460.500000000001</v>
       </c>
       <c r="P31" t="n">
-        <v>374.4</v>
+        <v>375.4</v>
       </c>
       <c r="Q31" t="n">
         <v>27.9</v>
@@ -3292,7 +3292,7 @@
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>374.4 (±27.9)</t>
+          <t>375.4 (±27.9)</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
@@ -3304,14 +3304,14 @@
         <v>197790</v>
       </c>
       <c r="X31" t="n">
-        <v>189.3</v>
+        <v>189.8</v>
       </c>
       <c r="Y31" t="n">
         <v>14.1</v>
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>189.3(±14.1)</t>
+          <t>189.8(±14.1)</t>
         </is>
       </c>
     </row>
@@ -3514,7 +3514,7 @@
         <v>2020</v>
       </c>
       <c r="D34" t="n">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="E34" t="n">
         <v>1701</v>
@@ -3550,7 +3550,7 @@
         <v>1710.9</v>
       </c>
       <c r="P34" t="n">
-        <v>300.4</v>
+        <v>299.4</v>
       </c>
       <c r="Q34" t="n">
         <v>43.3</v>
@@ -3568,7 +3568,7 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>300.4 (±43.3)</t>
+          <t>299.4 (±43.3)</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
@@ -3580,14 +3580,14 @@
         <v>109971</v>
       </c>
       <c r="X34" t="n">
-        <v>273.2</v>
+        <v>272.3</v>
       </c>
       <c r="Y34" t="n">
         <v>39.3</v>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>273.2(±39.3)</t>
+          <t>272.3(±39.3)</t>
         </is>
       </c>
     </row>
@@ -3606,7 +3606,7 @@
         <v>2020</v>
       </c>
       <c r="D35" t="n">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="E35" t="n">
         <v>807</v>
@@ -3642,13 +3642,13 @@
         <v>856</v>
       </c>
       <c r="P35" t="n">
-        <v>217.6</v>
+        <v>218.6</v>
       </c>
       <c r="Q35" t="n">
         <v>22.6</v>
       </c>
       <c r="R35" t="n">
-        <v>26.1</v>
+        <v>26.2</v>
       </c>
       <c r="S35" t="n">
         <v>3.3</v>
@@ -3660,26 +3660,26 @@
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>217.6 (±22.6)</t>
+          <t>218.6 (±22.6)</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>26.1% (±3.3%)</t>
+          <t>26.2% (±3.3%)</t>
         </is>
       </c>
       <c r="W35" t="n">
         <v>78102</v>
       </c>
       <c r="X35" t="n">
-        <v>278.6</v>
+        <v>279.9</v>
       </c>
       <c r="Y35" t="n">
         <v>28.9</v>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>278.6(±28.9)</t>
+          <t>279.9(±28.9)</t>
         </is>
       </c>
     </row>
@@ -3974,7 +3974,7 @@
         <v>2020</v>
       </c>
       <c r="D39" t="n">
-        <v>2228</v>
+        <v>2230</v>
       </c>
       <c r="E39" t="n">
         <v>1722</v>
@@ -4010,13 +4010,13 @@
         <v>1718.8</v>
       </c>
       <c r="P39" t="n">
-        <v>538.6</v>
+        <v>540.6</v>
       </c>
       <c r="Q39" t="n">
         <v>29.4</v>
       </c>
       <c r="R39" t="n">
-        <v>31.9</v>
+        <v>32</v>
       </c>
       <c r="S39" t="n">
         <v>2.3</v>
@@ -4028,26 +4028,26 @@
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>538.6 (±29.4)</t>
+          <t>540.6 (±29.4)</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>31.9% (±2.3%)</t>
+          <t>32.0% (±2.3%)</t>
         </is>
       </c>
       <c r="W39" t="n">
         <v>123715</v>
       </c>
       <c r="X39" t="n">
-        <v>435.4</v>
+        <v>437</v>
       </c>
       <c r="Y39" t="n">
         <v>23.7</v>
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>435.4(±23.7)</t>
+          <t>437.0(±23.7)</t>
         </is>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
         <v>2020</v>
       </c>
       <c r="D40" t="n">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="E40" t="n">
         <v>1064</v>
@@ -4102,13 +4102,13 @@
         <v>1060.1</v>
       </c>
       <c r="P40" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Q40" t="n">
         <v>24.1</v>
       </c>
       <c r="R40" t="n">
-        <v>22.9</v>
+        <v>23</v>
       </c>
       <c r="S40" t="n">
         <v>2.8</v>
@@ -4120,26 +4120,26 @@
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>237.0 (±24.1)</t>
+          <t>238.0 (±24.1)</t>
         </is>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>22.9% (±2.8%)</t>
+          <t>23.0% (±2.8%)</t>
         </is>
       </c>
       <c r="W40" t="n">
         <v>57932</v>
       </c>
       <c r="X40" t="n">
-        <v>409.1</v>
+        <v>410.8</v>
       </c>
       <c r="Y40" t="n">
         <v>41.6</v>
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>409.1(±41.6)</t>
+          <t>410.8(±41.6)</t>
         </is>
       </c>
     </row>
@@ -4894,7 +4894,7 @@
         <v>2020</v>
       </c>
       <c r="D49" t="n">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="E49" t="n">
         <v>1809</v>
@@ -4930,7 +4930,7 @@
         <v>1851.899999999999</v>
       </c>
       <c r="P49" t="n">
-        <v>471.8</v>
+        <v>470.8</v>
       </c>
       <c r="Q49" t="n">
         <v>17.7</v>
@@ -4948,7 +4948,7 @@
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>471.8 (±17.7)</t>
+          <t>470.8 (±17.7)</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
@@ -4960,14 +4960,14 @@
         <v>111249</v>
       </c>
       <c r="X49" t="n">
-        <v>424.1</v>
+        <v>423.2</v>
       </c>
       <c r="Y49" t="n">
         <v>15.9</v>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>424.1(±15.9)</t>
+          <t>423.2(±15.9)</t>
         </is>
       </c>
     </row>
@@ -4986,7 +4986,7 @@
         <v>2020</v>
       </c>
       <c r="D50" t="n">
-        <v>7850</v>
+        <v>7853</v>
       </c>
       <c r="E50" t="n">
         <v>6335</v>
@@ -5022,7 +5022,7 @@
         <v>6396.500000000001</v>
       </c>
       <c r="P50" t="n">
-        <v>1554.6</v>
+        <v>1557.6</v>
       </c>
       <c r="Q50" t="n">
         <v>101.1</v>
@@ -5031,7 +5031,7 @@
         <v>24.7</v>
       </c>
       <c r="S50" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="T50" t="inlineStr">
         <is>
@@ -5040,26 +5040,26 @@
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>1554.6 (±101.1)</t>
+          <t>1557.6 (±101.1)</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>24.7% (±2.0%)</t>
+          <t>24.7% (±1.9%)</t>
         </is>
       </c>
       <c r="W50" t="n">
         <v>637465</v>
       </c>
       <c r="X50" t="n">
-        <v>243.9</v>
+        <v>244.3</v>
       </c>
       <c r="Y50" t="n">
-        <v>15.8</v>
+        <v>15.9</v>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>243.9(±15.8)</t>
+          <t>244.3(±15.9)</t>
         </is>
       </c>
     </row>
@@ -5078,7 +5078,7 @@
         <v>2020</v>
       </c>
       <c r="D51" t="n">
-        <v>2684</v>
+        <v>2682</v>
       </c>
       <c r="E51" t="n">
         <v>2254</v>
@@ -5114,13 +5114,13 @@
         <v>2278.7</v>
       </c>
       <c r="P51" t="n">
-        <v>437.6</v>
+        <v>435.6</v>
       </c>
       <c r="Q51" t="n">
         <v>32.3</v>
       </c>
       <c r="R51" t="n">
-        <v>19.5</v>
+        <v>19.4</v>
       </c>
       <c r="S51" t="n">
         <v>1.7</v>
@@ -5132,26 +5132,26 @@
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>437.6 (±32.3)</t>
+          <t>435.6 (±32.3)</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>19.5% (±1.7%)</t>
+          <t>19.4% (±1.7%)</t>
         </is>
       </c>
       <c r="W51" t="n">
         <v>151611</v>
       </c>
       <c r="X51" t="n">
-        <v>288.6</v>
+        <v>287.3</v>
       </c>
       <c r="Y51" t="n">
         <v>21.3</v>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>288.6(±21.3)</t>
+          <t>287.3(±21.3)</t>
         </is>
       </c>
     </row>
@@ -5170,7 +5170,7 @@
         <v>2020</v>
       </c>
       <c r="D52" t="n">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="E52" t="n">
         <v>845</v>
@@ -5206,13 +5206,13 @@
         <v>826.2999999999998</v>
       </c>
       <c r="P52" t="n">
-        <v>162.4</v>
+        <v>163.4</v>
       </c>
       <c r="Q52" t="n">
         <v>33.7</v>
       </c>
       <c r="R52" t="n">
-        <v>20.5</v>
+        <v>20.6</v>
       </c>
       <c r="S52" t="n">
         <v>4.9</v>
@@ -5224,26 +5224,26 @@
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>162.4 (±33.7)</t>
+          <t>163.4 (±33.7)</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>20.5% (±4.9%)</t>
+          <t>20.6% (±4.9%)</t>
         </is>
       </c>
       <c r="W52" t="n">
         <v>54164</v>
       </c>
       <c r="X52" t="n">
-        <v>299.8</v>
+        <v>301.7</v>
       </c>
       <c r="Y52" t="n">
         <v>62.2</v>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>299.8(±62.2)</t>
+          <t>301.7(±62.2)</t>
         </is>
       </c>
     </row>
@@ -5262,7 +5262,7 @@
         <v>2020</v>
       </c>
       <c r="D53" t="n">
-        <v>3107</v>
+        <v>3108</v>
       </c>
       <c r="E53" t="n">
         <v>2658</v>
@@ -5298,7 +5298,7 @@
         <v>2688.400000000001</v>
       </c>
       <c r="P53" t="n">
-        <v>471.8</v>
+        <v>472.8</v>
       </c>
       <c r="Q53" t="n">
         <v>53.2</v>
@@ -5316,7 +5316,7 @@
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>471.8 (±53.2)</t>
+          <t>472.8 (±53.2)</t>
         </is>
       </c>
       <c r="V53" t="inlineStr">
@@ -5328,14 +5328,14 @@
         <v>228712</v>
       </c>
       <c r="X53" t="n">
-        <v>206.3</v>
+        <v>206.7</v>
       </c>
       <c r="Y53" t="n">
-        <v>23.2</v>
+        <v>23.3</v>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>206.3(±23.2)</t>
+          <t>206.7(±23.3)</t>
         </is>
       </c>
     </row>
@@ -5354,7 +5354,7 @@
         <v>2020</v>
       </c>
       <c r="D54" t="n">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="E54" t="n">
         <v>1749</v>
@@ -5390,13 +5390,13 @@
         <v>1782.7</v>
       </c>
       <c r="P54" t="n">
-        <v>297.4</v>
+        <v>296.4</v>
       </c>
       <c r="Q54" t="n">
         <v>43.1</v>
       </c>
       <c r="R54" t="n">
-        <v>17.1</v>
+        <v>17</v>
       </c>
       <c r="S54" t="n">
         <v>2.8</v>
@@ -5408,26 +5408,26 @@
       </c>
       <c r="U54" t="inlineStr">
         <is>
-          <t>297.4 (±43.1)</t>
+          <t>296.4 (±43.1)</t>
         </is>
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>17.1% (±2.8%)</t>
+          <t>17.0% (±2.8%)</t>
         </is>
       </c>
       <c r="W54" t="n">
         <v>112401</v>
       </c>
       <c r="X54" t="n">
-        <v>264.6</v>
+        <v>263.7</v>
       </c>
       <c r="Y54" t="n">
         <v>38.3</v>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>264.6(±38.3)</t>
+          <t>263.7(±38.3)</t>
         </is>
       </c>
     </row>
@@ -6182,7 +6182,7 @@
         <v>2020</v>
       </c>
       <c r="D63" t="n">
-        <v>1926</v>
+        <v>1927</v>
       </c>
       <c r="E63" t="n">
         <v>1546</v>
@@ -6218,16 +6218,16 @@
         <v>1571.3</v>
       </c>
       <c r="P63" t="n">
-        <v>360.2</v>
+        <v>361.2</v>
       </c>
       <c r="Q63" t="n">
         <v>5.5</v>
       </c>
       <c r="R63" t="n">
-        <v>23</v>
+        <v>23.1</v>
       </c>
       <c r="S63" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="T63" t="inlineStr">
         <is>
@@ -6236,26 +6236,26 @@
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>360.2 (±5.5)</t>
+          <t>361.2 (±5.5)</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>23.0% (±0.4%)</t>
+          <t>23.1% (±0.5%)</t>
         </is>
       </c>
       <c r="W63" t="n">
         <v>158204</v>
       </c>
       <c r="X63" t="n">
-        <v>227.7</v>
+        <v>228.3</v>
       </c>
       <c r="Y63" t="n">
         <v>3.5</v>
       </c>
       <c r="Z63" t="inlineStr">
         <is>
-          <t>227.7(±3.5)</t>
+          <t>228.3(±3.5)</t>
         </is>
       </c>
     </row>
@@ -6458,7 +6458,7 @@
         <v>2020</v>
       </c>
       <c r="D66" t="n">
-        <v>2721</v>
+        <v>2722</v>
       </c>
       <c r="E66" t="n">
         <v>2429</v>
@@ -6494,13 +6494,13 @@
         <v>2405.1</v>
       </c>
       <c r="P66" t="n">
-        <v>397.8</v>
+        <v>398.8</v>
       </c>
       <c r="Q66" t="n">
         <v>81.90000000000001</v>
       </c>
       <c r="R66" t="n">
-        <v>17.1</v>
+        <v>17.2</v>
       </c>
       <c r="S66" t="n">
         <v>4</v>
@@ -6512,26 +6512,26 @@
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>397.8 (±81.9)</t>
+          <t>398.8 (±81.9)</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>17.1% (±4.0%)</t>
+          <t>17.2% (±4.0%)</t>
         </is>
       </c>
       <c r="W66" t="n">
         <v>127001</v>
       </c>
       <c r="X66" t="n">
-        <v>313.2</v>
+        <v>314</v>
       </c>
       <c r="Y66" t="n">
         <v>64.5</v>
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>313.2(±64.5)</t>
+          <t>314.0(±64.5)</t>
         </is>
       </c>
     </row>
@@ -6550,7 +6550,7 @@
         <v>2020</v>
       </c>
       <c r="D67" t="n">
-        <v>4136</v>
+        <v>4139</v>
       </c>
       <c r="E67" t="n">
         <v>3326</v>
@@ -6586,16 +6586,16 @@
         <v>3315.3</v>
       </c>
       <c r="P67" t="n">
-        <v>887.8</v>
+        <v>890.8</v>
       </c>
       <c r="Q67" t="n">
         <v>67.09999999999999</v>
       </c>
       <c r="R67" t="n">
-        <v>27.3</v>
+        <v>27.4</v>
       </c>
       <c r="S67" t="n">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="T67" t="inlineStr">
         <is>
@@ -6604,26 +6604,26 @@
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>887.8 (±67.1)</t>
+          <t>890.8 (±67.1)</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>27.3% (±2.5%)</t>
+          <t>27.4% (±2.6%)</t>
         </is>
       </c>
       <c r="W67" t="n">
         <v>252776</v>
       </c>
       <c r="X67" t="n">
-        <v>351.2</v>
+        <v>352.4</v>
       </c>
       <c r="Y67" t="n">
         <v>26.6</v>
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>351.2(±26.6)</t>
+          <t>352.4(±26.6)</t>
         </is>
       </c>
     </row>
@@ -6642,7 +6642,7 @@
         <v>2020</v>
       </c>
       <c r="D68" t="n">
-        <v>2342</v>
+        <v>2343</v>
       </c>
       <c r="E68" t="n">
         <v>2003</v>
@@ -6678,7 +6678,7 @@
         <v>1998.1</v>
       </c>
       <c r="P68" t="n">
-        <v>383.6</v>
+        <v>384.6</v>
       </c>
       <c r="Q68" t="n">
         <v>39.7</v>
@@ -6687,7 +6687,7 @@
         <v>19.6</v>
       </c>
       <c r="S68" t="n">
-        <v>2.4</v>
+        <v>2.3</v>
       </c>
       <c r="T68" t="inlineStr">
         <is>
@@ -6696,26 +6696,26 @@
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>383.6 (±39.7)</t>
+          <t>384.6 (±39.7)</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>19.6% (±2.4%)</t>
+          <t>19.6% (±2.3%)</t>
         </is>
       </c>
       <c r="W68" t="n">
         <v>119190</v>
       </c>
       <c r="X68" t="n">
-        <v>321.8</v>
+        <v>322.7</v>
       </c>
       <c r="Y68" t="n">
         <v>33.3</v>
       </c>
       <c r="Z68" t="inlineStr">
         <is>
-          <t>321.8(±33.3)</t>
+          <t>322.7(±33.3)</t>
         </is>
       </c>
     </row>
@@ -6826,7 +6826,7 @@
         <v>2020</v>
       </c>
       <c r="D70" t="n">
-        <v>9905</v>
+        <v>9904</v>
       </c>
       <c r="E70" t="n">
         <v>8132</v>
@@ -6862,7 +6862,7 @@
         <v>8172.5</v>
       </c>
       <c r="P70" t="n">
-        <v>1882.4</v>
+        <v>1881.4</v>
       </c>
       <c r="Q70" t="n">
         <v>149.9</v>
@@ -6880,7 +6880,7 @@
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>1882.4 (±149.9)</t>
+          <t>1881.4 (±149.9)</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
@@ -6892,14 +6892,14 @@
         <v>666801</v>
       </c>
       <c r="X70" t="n">
-        <v>282.3</v>
+        <v>282.2</v>
       </c>
       <c r="Y70" t="n">
-        <v>22.5</v>
+        <v>22.4</v>
       </c>
       <c r="Z70" t="inlineStr">
         <is>
-          <t>282.3(±22.5)</t>
+          <t>282.2(±22.4)</t>
         </is>
       </c>
     </row>
@@ -6918,7 +6918,7 @@
         <v>2020</v>
       </c>
       <c r="D71" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E71" t="n">
         <v>1580</v>
@@ -6954,7 +6954,7 @@
         <v>1586.299999999999</v>
       </c>
       <c r="P71" t="n">
-        <v>464.6</v>
+        <v>465.6</v>
       </c>
       <c r="Q71" t="n">
         <v>29.9</v>
@@ -6963,7 +6963,7 @@
         <v>29.9</v>
       </c>
       <c r="S71" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="T71" t="inlineStr">
         <is>
@@ -6972,26 +6972,26 @@
       </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>464.6 (±29.9)</t>
+          <t>465.6 (±29.9)</t>
         </is>
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>29.9% (±2.5%)</t>
+          <t>29.9% (±2.4%)</t>
         </is>
       </c>
       <c r="W71" t="n">
         <v>110789</v>
       </c>
       <c r="X71" t="n">
-        <v>419.4</v>
+        <v>420.3</v>
       </c>
       <c r="Y71" t="n">
         <v>26.9</v>
       </c>
       <c r="Z71" t="inlineStr">
         <is>
-          <t>419.4(±26.9)</t>
+          <t>420.3(±26.9)</t>
         </is>
       </c>
     </row>
@@ -7286,7 +7286,7 @@
         <v>2020</v>
       </c>
       <c r="D75" t="n">
-        <v>2798</v>
+        <v>2799</v>
       </c>
       <c r="E75" t="n">
         <v>2380</v>
@@ -7322,16 +7322,16 @@
         <v>2381.900000000001</v>
       </c>
       <c r="P75" t="n">
-        <v>474.6</v>
+        <v>475.6</v>
       </c>
       <c r="Q75" t="n">
         <v>58.5</v>
       </c>
       <c r="R75" t="n">
-        <v>20.4</v>
+        <v>20.5</v>
       </c>
       <c r="S75" t="n">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="T75" t="inlineStr">
         <is>
@@ -7340,26 +7340,26 @@
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>474.6 (±58.5)</t>
+          <t>475.6 (±58.5)</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>20.4% (±2.9%)</t>
+          <t>20.5% (±3.0%)</t>
         </is>
       </c>
       <c r="W75" t="n">
         <v>184119</v>
       </c>
       <c r="X75" t="n">
-        <v>257.8</v>
+        <v>258.3</v>
       </c>
       <c r="Y75" t="n">
-        <v>31.7</v>
+        <v>31.8</v>
       </c>
       <c r="Z75" t="inlineStr">
         <is>
-          <t>257.8(±31.7)</t>
+          <t>258.3(±31.8)</t>
         </is>
       </c>
     </row>
@@ -7470,7 +7470,7 @@
         <v>2020</v>
       </c>
       <c r="D77" t="n">
-        <v>4178</v>
+        <v>4177</v>
       </c>
       <c r="E77" t="n">
         <v>3458</v>
@@ -7506,7 +7506,7 @@
         <v>3525.599999999999</v>
       </c>
       <c r="P77" t="n">
-        <v>700.4</v>
+        <v>699.4</v>
       </c>
       <c r="Q77" t="n">
         <v>48</v>
@@ -7524,7 +7524,7 @@
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>700.4 (±48.0)</t>
+          <t>699.4 (±48.0)</t>
         </is>
       </c>
       <c r="V77" t="inlineStr">
@@ -7536,14 +7536,14 @@
         <v>226671</v>
       </c>
       <c r="X77" t="n">
-        <v>309</v>
+        <v>308.6</v>
       </c>
       <c r="Y77" t="n">
-        <v>21.2</v>
+        <v>21.1</v>
       </c>
       <c r="Z77" t="inlineStr">
         <is>
-          <t>309.0(±21.2)</t>
+          <t>308.6(±21.1)</t>
         </is>
       </c>
     </row>
@@ -7562,7 +7562,7 @@
         <v>2020</v>
       </c>
       <c r="D78" t="n">
-        <v>15133</v>
+        <v>15141</v>
       </c>
       <c r="E78" t="n">
         <v>12899</v>
@@ -7598,16 +7598,16 @@
         <v>12980.1</v>
       </c>
       <c r="P78" t="n">
-        <v>2356.6</v>
+        <v>2364.6</v>
       </c>
       <c r="Q78" t="n">
         <v>203.7</v>
       </c>
       <c r="R78" t="n">
-        <v>18.4</v>
+        <v>18.5</v>
       </c>
       <c r="S78" t="n">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T78" t="inlineStr">
         <is>
@@ -7616,26 +7616,26 @@
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>2356.6 (±203.7)</t>
+          <t>2364.6 (±203.7)</t>
         </is>
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>18.4% (±1.8%)</t>
+          <t>18.5% (±1.9%)</t>
         </is>
       </c>
       <c r="W78" t="n">
         <v>1328790</v>
       </c>
       <c r="X78" t="n">
-        <v>177.3</v>
+        <v>178</v>
       </c>
       <c r="Y78" t="n">
-        <v>15.4</v>
+        <v>15.3</v>
       </c>
       <c r="Z78" t="inlineStr">
         <is>
-          <t>177.3(±15.4)</t>
+          <t>178.0(±15.3)</t>
         </is>
       </c>
     </row>
@@ -7654,7 +7654,7 @@
         <v>2020</v>
       </c>
       <c r="D79" t="n">
-        <v>5047</v>
+        <v>5045</v>
       </c>
       <c r="E79" t="n">
         <v>4332</v>
@@ -7690,16 +7690,16 @@
         <v>4353.9</v>
       </c>
       <c r="P79" t="n">
-        <v>768.2</v>
+        <v>766.2</v>
       </c>
       <c r="Q79" t="n">
         <v>75.09999999999999</v>
       </c>
       <c r="R79" t="n">
-        <v>18</v>
+        <v>17.9</v>
       </c>
       <c r="S79" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="T79" t="inlineStr">
         <is>
@@ -7708,26 +7708,26 @@
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>768.2 (±75.1)</t>
+          <t>766.2 (±75.1)</t>
         </is>
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>18.0% (±2.1%)</t>
+          <t>17.9% (±2.0%)</t>
         </is>
       </c>
       <c r="W79" t="n">
         <v>313396</v>
       </c>
       <c r="X79" t="n">
-        <v>245.1</v>
+        <v>244.5</v>
       </c>
       <c r="Y79" t="n">
-        <v>24</v>
+        <v>23.9</v>
       </c>
       <c r="Z79" t="inlineStr">
         <is>
-          <t>245.1(±24.0)</t>
+          <t>244.5(±23.9)</t>
         </is>
       </c>
     </row>
@@ -7746,7 +7746,7 @@
         <v>2020</v>
       </c>
       <c r="D80" t="n">
-        <v>1844</v>
+        <v>1846</v>
       </c>
       <c r="E80" t="n">
         <v>1549</v>
@@ -7782,13 +7782,13 @@
         <v>1553.6</v>
       </c>
       <c r="P80" t="n">
-        <v>319.8</v>
+        <v>321.8</v>
       </c>
       <c r="Q80" t="n">
         <v>29.4</v>
       </c>
       <c r="R80" t="n">
-        <v>21</v>
+        <v>21.1</v>
       </c>
       <c r="S80" t="n">
         <v>2.3</v>
@@ -7800,26 +7800,26 @@
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>319.8 (±29.4)</t>
+          <t>321.8 (±29.4)</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>21.0% (±2.3%)</t>
+          <t>21.1% (±2.3%)</t>
         </is>
       </c>
       <c r="W80" t="n">
         <v>110914</v>
       </c>
       <c r="X80" t="n">
-        <v>288.3</v>
+        <v>290.1</v>
       </c>
       <c r="Y80" t="n">
         <v>26.5</v>
       </c>
       <c r="Z80" t="inlineStr">
         <is>
-          <t>288.3(±26.5)</t>
+          <t>290.1(±26.5)</t>
         </is>
       </c>
     </row>
@@ -7838,7 +7838,7 @@
         <v>2020</v>
       </c>
       <c r="D81" t="n">
-        <v>5892</v>
+        <v>5893</v>
       </c>
       <c r="E81" t="n">
         <v>4985</v>
@@ -7874,7 +7874,7 @@
         <v>5083.4</v>
       </c>
       <c r="P81" t="n">
-        <v>905.4</v>
+        <v>906.4</v>
       </c>
       <c r="Q81" t="n">
         <v>96.8</v>
@@ -7892,7 +7892,7 @@
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>905.4 (±96.8)</t>
+          <t>906.4 (±96.8)</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
@@ -7904,14 +7904,14 @@
         <v>469885</v>
       </c>
       <c r="X81" t="n">
-        <v>192.7</v>
+        <v>192.9</v>
       </c>
       <c r="Y81" t="n">
         <v>20.6</v>
       </c>
       <c r="Z81" t="inlineStr">
         <is>
-          <t>192.7(±20.6)</t>
+          <t>192.9(±20.6)</t>
         </is>
       </c>
     </row>
@@ -7930,7 +7930,7 @@
         <v>2020</v>
       </c>
       <c r="D82" t="n">
-        <v>3827</v>
+        <v>3826</v>
       </c>
       <c r="E82" t="n">
         <v>3357</v>
@@ -7966,7 +7966,7 @@
         <v>3400.2</v>
       </c>
       <c r="P82" t="n">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Q82" t="n">
         <v>40.2</v>
@@ -7975,7 +7975,7 @@
         <v>13.9</v>
       </c>
       <c r="S82" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="T82" t="inlineStr">
         <is>
@@ -7984,26 +7984,26 @@
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>467.0 (±40.2)</t>
+          <t>466.0 (±40.2)</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>13.9% (±1.3%)</t>
+          <t>13.9% (±1.4%)</t>
         </is>
       </c>
       <c r="W82" t="n">
         <v>232568</v>
       </c>
       <c r="X82" t="n">
-        <v>200.8</v>
+        <v>200.4</v>
       </c>
       <c r="Y82" t="n">
         <v>17.3</v>
       </c>
       <c r="Z82" t="inlineStr">
         <is>
-          <t>200.8(±17.3)</t>
+          <t>200.4(±17.3)</t>
         </is>
       </c>
     </row>

</xml_diff>